<commit_message>
revise hw2 of Data Structure
</commit_message>
<xml_diff>
--- a/DataStructure_HW/HW2/hw2_OriginalData_diagram.xlsx
+++ b/DataStructure_HW/HW2/hw2_OriginalData_diagram.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywt01\Documents\codes\nccu_cs_hw\DataStructure_HW\HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0218093A-2C4B-431B-B372-A4AA1E837DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F4FB7-E50B-43FD-B768-544785802D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insert_t" sheetId="1" r:id="rId1"/>
     <sheet name="insert_t2" sheetId="4" r:id="rId2"/>
     <sheet name="search_t" sheetId="2" r:id="rId3"/>
-    <sheet name="skip_list_number" sheetId="3" r:id="rId4"/>
+    <sheet name="skip list_copy number" sheetId="5" r:id="rId4"/>
+    <sheet name="skip list_list_number" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -32,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
-  <si>
-    <t>k</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>sorted_array</t>
   </si>
@@ -52,58 +50,11 @@
     <t>Skip List_0.9</t>
   </si>
   <si>
-    <t>k=10</t>
-  </si>
-  <si>
-    <t>k=11</t>
-  </si>
-  <si>
-    <t>k=12</t>
-  </si>
-  <si>
-    <t>k=13</t>
-  </si>
-  <si>
-    <t>k=14</t>
-  </si>
-  <si>
-    <t>k=15</t>
-  </si>
-  <si>
-    <t>k=16</t>
-  </si>
-  <si>
-    <t>k=17</t>
-  </si>
-  <si>
-    <t>k=18</t>
-  </si>
-  <si>
-    <t>k=19</t>
-  </si>
-  <si>
-    <t>k=20</t>
-  </si>
-  <si>
-    <t>k=21</t>
-  </si>
-  <si>
-    <t>k=22</t>
-  </si>
-  <si>
     <t>趨勢線</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Skip List_0.9</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>y = 2E-08x1.244</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>y = 5E-08x2.1214</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -277,7 +228,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -289,6 +240,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1635,6 +1589,917 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-TW" altLang="en-US"/>
+              <a:t>圖七</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'skip list_copy number'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Skip List_0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'skip list_copy number'!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>268435456</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>536870912</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1073741824</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'skip list_copy number'!$C$2:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1.1123000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.11182</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.11182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.10938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1097399999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1106</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.11103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1116299999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1115900000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.11148</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1114999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1115900000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1115699999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1115600000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA69-4311-B59B-4821D8D75B46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'skip list_copy number'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Skip List_0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'skip list_copy number'!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>268435456</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>536870912</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1073741824</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'skip list_copy number'!$D$2:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1.9355500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9565399999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0019499999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.00061</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9989300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0003500000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9974400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9946200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9947999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA69-4311-B59B-4821D8D75B46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'skip list_copy number'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Skip List_0.9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'skip list_copy number'!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>268435456</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>536870912</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1073741824</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'skip list_copy number'!$E$2:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>9.8632799999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8740199999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0405</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9879200000000008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9829699999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9491300000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.9352499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9272200000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9206599999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AA69-4311-B59B-4821D8D75B46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1436037008"/>
+        <c:axId val="1436037424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1436037008"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>資料量</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1436037424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1436037424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>平均每個</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>data</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>的
+</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>additional copy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>個數
+</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>平均層數</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1436037008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -2754,6 +3619,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>時間</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4020,6 +4945,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>資料量</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4082,6 +5062,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>時間</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5347,6 +6386,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>資料量</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5409,6 +6503,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>時間</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5546,12 +6700,271 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-TW" altLang="en-US"/>
+              <a:t>原始資料</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>skip list_0.1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="zh-TW"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>insert_t2!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>268435456</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>536870912</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1073741824</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>insert_t2!$C$2:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>8.0599999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0500000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.3280000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1735000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4823999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2084999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11432100000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25639699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63947399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.64184</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.13809</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.558800000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.918999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>296.28100000000001</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF14-48F4-AC5A-9A8576FABDF4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -5939,226 +7352,7 @@
         </c:dLbls>
         <c:axId val="1708184863"/>
         <c:axId val="1708185279"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:tx>
-                  <c:v>skip list_0.1</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="25400" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:trendline>
-                  <c:spPr>
-                    <a:ln w="19050" cap="rnd">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                      <a:prstDash val="sysDot"/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:trendlineType val="power"/>
-                  <c:dispRSqr val="0"/>
-                  <c:dispEq val="1"/>
-                  <c:trendlineLbl>
-                    <c:numFmt formatCode="General" sourceLinked="0"/>
-                    <c:spPr>
-                      <a:noFill/>
-                      <a:ln>
-                        <a:noFill/>
-                      </a:ln>
-                      <a:effectLst/>
-                    </c:spPr>
-                    <c:txPr>
-                      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                      <a:lstStyle/>
-                      <a:p>
-                        <a:pPr>
-                          <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="65000"/>
-                                <a:lumOff val="35000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                            <a:latin typeface="+mn-lt"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:defRPr>
-                        </a:pPr>
-                        <a:endParaRPr lang="zh-TW"/>
-                      </a:p>
-                    </c:txPr>
-                  </c:trendlineLbl>
-                </c:trendline>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>insert_t2!$B$2:$B$22</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="21"/>
-                      <c:pt idx="0">
-                        <c:v>1024</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2048</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>4096</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>8192</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>16384</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>32768</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>65536</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>131072</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>262144</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>524288</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1048576</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>2097152</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>4194304</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>8388608</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>16777216</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>33554432</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>67108864</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>134217728</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>268435456</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>536870912</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>1073741824</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>insert_t2!$C$2:$C$15</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="14"/>
-                      <c:pt idx="0">
-                        <c:v>8.0599999999999997E-4</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>2.0500000000000002E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>5.3280000000000003E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1.1735000000000001E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>2.4823999999999999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>5.2084999999999999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0.11432100000000001</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0.25639699999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0.63947399999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1.64184</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>5.13809</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>16.558800000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>49.918999999999997</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>296.28100000000001</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-FF14-48F4-AC5A-9A8576FABDF4}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1708184863"/>
@@ -7041,6 +8235,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>資料量</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7103,6 +8352,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>時間</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9670,8 +10979,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>時間</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -10870,6 +12239,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>資料量 </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -10932,6 +12356,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-TW" altLang="en-US"/>
+                  <a:t>時間</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>(s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -11054,6 +12538,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -11929,7 +13453,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12445,7 +13969,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12961,7 +14485,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13477,7 +15001,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13993,7 +15517,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14509,7 +16033,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15025,7 +16549,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15541,7 +17065,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16057,20 +17581,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>139342</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>79073</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>275414</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>65466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>113034</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>200871</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99427</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16097,16 +18137,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>201706</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>89648</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>283349</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>81485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>392206</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>433028</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -16121,10 +18161,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3657920" y="4335077"/>
-          <a:ext cx="11593286" cy="7162959"/>
-          <a:chOff x="3440206" y="4988219"/>
-          <a:chExt cx="11593286" cy="8278745"/>
+          <a:off x="978674" y="4710635"/>
+          <a:ext cx="11608254" cy="7290866"/>
+          <a:chOff x="3440206" y="5101846"/>
+          <a:chExt cx="11593286" cy="8697542"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:graphicFrame macro="">
@@ -16139,7 +18179,7 @@
           <xdr:cNvGraphicFramePr/>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
-          <a:off x="6086391" y="4988219"/>
+          <a:off x="6086391" y="5101846"/>
           <a:ext cx="7029292" cy="5261962"/>
         </xdr:xfrm>
         <a:graphic>
@@ -16161,10 +18201,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="3440206" y="9936486"/>
-            <a:ext cx="11593286" cy="3330478"/>
+            <a:off x="3440206" y="9936487"/>
+            <a:ext cx="11593286" cy="3862901"/>
             <a:chOff x="3630706" y="10056549"/>
-            <a:chExt cx="11620500" cy="3480157"/>
+            <a:chExt cx="11620500" cy="4036508"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:graphicFrame macro="">
@@ -16182,7 +18222,7 @@
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
             <a:off x="3630706" y="11116236"/>
-            <a:ext cx="5586133" cy="2420470"/>
+            <a:ext cx="5586133" cy="2976821"/>
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16205,7 +18245,7 @@
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
             <a:off x="9827559" y="11071413"/>
-            <a:ext cx="5423647" cy="2420470"/>
+            <a:ext cx="5423647" cy="2962279"/>
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16449,16 +18489,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16485,16 +18525,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16526,16 +18566,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>209549</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16562,16 +18602,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1200151</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1000124</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -16586,10 +18626,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7458076" y="5219700"/>
-          <a:ext cx="6391274" cy="6800850"/>
-          <a:chOff x="7458076" y="5219700"/>
-          <a:chExt cx="6391274" cy="6800850"/>
+          <a:off x="628650" y="5162550"/>
+          <a:ext cx="6629399" cy="7115175"/>
+          <a:chOff x="7458075" y="5248275"/>
+          <a:chExt cx="6629399" cy="6772275"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:graphicFrame macro="">
@@ -16604,8 +18644,8 @@
           <xdr:cNvGraphicFramePr/>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
-          <a:off x="7458076" y="5219700"/>
-          <a:ext cx="6343650" cy="3143250"/>
+          <a:off x="7458075" y="5248275"/>
+          <a:ext cx="6629399" cy="3143250"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -16768,6 +18808,47 @@
         </xdr:style>
       </xdr:cxnSp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>585786</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D241E4-8A4D-4F6B-8E6C-9F504083306B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -17644,8 +19725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G22"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -17662,25 +19743,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -18235,22 +20316,22 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="F23" s="6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -18263,10 +20344,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ED08B7-CD6E-4DCE-8E0B-BFD57E76B928}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -18281,30 +20362,24 @@
     <col min="8" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:5">
       <c r="A2" s="4">
         <v>10</v>
       </c>
@@ -18321,14 +20396,8 @@
       <c r="E2" s="6">
         <v>1.5510000000000001E-3</v>
       </c>
-      <c r="F2" s="6">
-        <v>0.116163</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1.5799999999999999E-4</v>
-      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:5">
       <c r="A3" s="4">
         <v>11</v>
       </c>
@@ -18345,14 +20414,8 @@
       <c r="E3" s="6">
         <v>4.4759999999999999E-3</v>
       </c>
-      <c r="F3" s="6">
-        <v>0.51663599999999998</v>
-      </c>
-      <c r="G3" s="6">
-        <v>3.0400000000000002E-4</v>
-      </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5">
       <c r="A4" s="4">
         <v>12</v>
       </c>
@@ -18369,14 +20432,8 @@
       <c r="E4" s="6">
         <v>1.0451999999999999E-2</v>
       </c>
-      <c r="F4" s="6">
-        <v>2.42442</v>
-      </c>
-      <c r="G4" s="6">
-        <v>7.4799999999999997E-4</v>
-      </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
         <v>13</v>
       </c>
@@ -18393,14 +20450,8 @@
       <c r="E5" s="6">
         <v>2.4365999999999999E-2</v>
       </c>
-      <c r="F5" s="6">
-        <v>10.402900000000001</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1.8990000000000001E-3</v>
-      </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
         <v>14</v>
       </c>
@@ -18417,14 +20468,8 @@
       <c r="E6" s="6">
         <v>5.1083000000000003E-2</v>
       </c>
-      <c r="F6" s="6">
-        <v>46.3294</v>
-      </c>
-      <c r="G6" s="6">
-        <v>3.8430000000000001E-3</v>
-      </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:5">
       <c r="A7" s="4">
         <v>15</v>
       </c>
@@ -18441,14 +20486,8 @@
       <c r="E7" s="6">
         <v>0.130241</v>
       </c>
-      <c r="F7" s="6">
-        <v>191.083</v>
-      </c>
-      <c r="G7" s="6">
-        <v>8.3940000000000004E-3</v>
-      </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:5">
       <c r="A8" s="4">
         <v>16</v>
       </c>
@@ -18465,14 +20504,8 @@
       <c r="E8" s="6">
         <v>0.365587</v>
       </c>
-      <c r="F8" s="6">
-        <v>819.38699999999994</v>
-      </c>
-      <c r="G8" s="6">
-        <v>2.3576E-2</v>
-      </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:5">
       <c r="A9" s="4">
         <v>17</v>
       </c>
@@ -18489,14 +20522,8 @@
       <c r="E9" s="6">
         <v>1.0285</v>
       </c>
-      <c r="F9" s="6">
-        <v>3708.27</v>
-      </c>
-      <c r="G9" s="6">
-        <v>5.8011E-2</v>
-      </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
         <v>18</v>
       </c>
@@ -18513,14 +20540,8 @@
       <c r="E10" s="6">
         <v>2.4959199999999999</v>
       </c>
-      <c r="F10" s="6">
-        <v>14847.9</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0.108416</v>
-      </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
         <v>19</v>
       </c>
@@ -18538,15 +20559,8 @@
         <f t="shared" ref="E11:E22" si="1" xml:space="preserve"> 0.0000002 * B11^1.3136</f>
         <v>6.5201417786181075</v>
       </c>
-      <c r="F11" s="8">
-        <f xml:space="preserve"> 0.00000005*B11^2.1214</f>
-        <v>67993.222932839752</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.30029099999999997</v>
-      </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
         <v>20</v>
       </c>
@@ -18565,15 +20579,8 @@
         <f t="shared" si="1"/>
         <v>16.206530159341373</v>
       </c>
-      <c r="F12" s="8">
-        <f t="shared" ref="F12:F22" si="3" xml:space="preserve"> 0.00000005*B12^2.1214</f>
-        <v>295849.37787965656</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0.90643799999999997</v>
-      </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:5">
       <c r="A13" s="4">
         <v>21</v>
       </c>
@@ -18592,15 +20599,8 @@
         <f t="shared" si="1"/>
         <v>40.283114803879066</v>
       </c>
-      <c r="F13" s="8">
-        <f t="shared" si="3"/>
-        <v>1287287.9180655209</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1.6945699999999999</v>
-      </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:5">
       <c r="A14" s="4">
         <v>22</v>
       </c>
@@ -18619,15 +20619,8 @@
         <f t="shared" si="1"/>
         <v>100.12811640418703</v>
       </c>
-      <c r="F14" s="8">
-        <f t="shared" si="3"/>
-        <v>5601195.4321956523</v>
-      </c>
-      <c r="G14" s="6">
-        <v>4.2556900000000004</v>
-      </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:5">
       <c r="A15" s="4">
         <v>23</v>
       </c>
@@ -18646,15 +20639,8 @@
         <f t="shared" si="1"/>
         <v>248.87945590754089</v>
       </c>
-      <c r="F15" s="8">
-        <f t="shared" si="3"/>
-        <v>24371696.362066362</v>
-      </c>
-      <c r="G15" s="6">
-        <v>11.7082</v>
-      </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:5">
       <c r="A16" s="4">
         <v>24</v>
       </c>
@@ -18663,7 +20649,7 @@
         <v>16777216</v>
       </c>
       <c r="C16" s="8">
-        <f t="shared" ref="C16:C22" si="4" xml:space="preserve">  0.00000006 * B16^1.3378</f>
+        <f t="shared" ref="C16:C22" si="3" xml:space="preserve">  0.00000006 * B16^1.3378</f>
         <v>277.57575334224686</v>
       </c>
       <c r="D16" s="8">
@@ -18674,15 +20660,8 @@
         <f t="shared" si="1"/>
         <v>618.61728550646569</v>
       </c>
-      <c r="F16" s="8">
-        <f t="shared" si="3"/>
-        <v>106045145.31854504</v>
-      </c>
-      <c r="G16" s="6">
-        <v>23.907399999999999</v>
-      </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:5">
       <c r="A17" s="4">
         <v>25</v>
       </c>
@@ -18691,7 +20670,7 @@
         <v>33554432</v>
       </c>
       <c r="C17" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>701.61595319380649</v>
       </c>
       <c r="D17" s="8">
@@ -18702,15 +20681,8 @@
         <f t="shared" si="1"/>
         <v>1537.6413634942949</v>
       </c>
-      <c r="F17" s="8">
-        <f t="shared" si="3"/>
-        <v>461419372.64304388</v>
-      </c>
-      <c r="G17" s="6">
-        <v>53.217100000000002</v>
-      </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:5">
       <c r="A18" s="4">
         <v>26</v>
       </c>
@@ -18719,7 +20691,7 @@
         <v>67108864</v>
       </c>
       <c r="C18" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1773.4436089923702</v>
       </c>
       <c r="D18" s="8">
@@ -18730,15 +20702,8 @@
         <f t="shared" si="1"/>
         <v>3821.9768799264593</v>
       </c>
-      <c r="F18" s="8">
-        <f t="shared" si="3"/>
-        <v>2007709422.3479192</v>
-      </c>
-      <c r="G18" s="6">
-        <v>123.15600000000001</v>
-      </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:5">
       <c r="A19" s="4">
         <v>27</v>
       </c>
@@ -18747,7 +20712,7 @@
         <v>134217728</v>
       </c>
       <c r="C19" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4482.6549623895698</v>
       </c>
       <c r="D19" s="8">
@@ -18758,16 +20723,8 @@
         <f t="shared" si="1"/>
         <v>9499.9442766659777</v>
       </c>
-      <c r="F19" s="8">
-        <f t="shared" si="3"/>
-        <v>8735864516.2542667</v>
-      </c>
-      <c r="G19" s="8">
-        <f>0.00000002*B19^1.244</f>
-        <v>258.24117555594438</v>
-      </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:5">
       <c r="A20" s="4">
         <v>28</v>
       </c>
@@ -18776,7 +20733,7 @@
         <v>268435456</v>
       </c>
       <c r="C20" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11330.608658739791</v>
       </c>
       <c r="D20" s="8">
@@ -18787,16 +20744,8 @@
         <f t="shared" si="1"/>
         <v>23613.157299238959</v>
       </c>
-      <c r="F20" s="8">
-        <f t="shared" si="3"/>
-        <v>38011142447.646744</v>
-      </c>
-      <c r="G20" s="8">
-        <f>0.00000002*B20^1.244</f>
-        <v>611.65538644522962</v>
-      </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:5">
       <c r="A21" s="4">
         <v>29</v>
       </c>
@@ -18805,7 +20754,7 @@
         <v>536870912</v>
       </c>
       <c r="C21" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28639.878298612803</v>
       </c>
       <c r="D21" s="8">
@@ -18816,16 +20765,8 @@
         <f t="shared" si="1"/>
         <v>58693.101917255699</v>
       </c>
-      <c r="F21" s="8">
-        <f t="shared" si="3"/>
-        <v>165392554736.50925</v>
-      </c>
-      <c r="G21" s="8">
-        <f>0.00000002*B21^1.244</f>
-        <v>1448.7322208089008</v>
-      </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:5">
       <c r="A22" s="4">
         <v>30</v>
       </c>
@@ -18834,7 +20775,7 @@
         <v>1073741824</v>
       </c>
       <c r="C22" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>72391.753493900862</v>
       </c>
       <c r="D22" s="8">
@@ -18845,33 +20786,19 @@
         <f t="shared" si="1"/>
         <v>145888.16603446615</v>
       </c>
-      <c r="F22" s="8">
-        <f t="shared" si="3"/>
-        <v>719649434371.64526</v>
-      </c>
-      <c r="G22" s="8">
-        <f>0.00000002*B22^1.244</f>
-        <v>3431.3848845632951</v>
-      </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -18886,8 +20813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737C9493-ED4E-44AB-B916-0A25225F2F82}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -18901,25 +20828,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -19474,22 +21401,22 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -19500,34 +21427,369 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DF60A9-7E88-4278-B172-EDB855FE47DA}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <f>POWER(2,A2)</f>
+        <v>1024</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1.1123000000000001</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1.9355500000000001</v>
+      </c>
+      <c r="E2" s="5">
+        <v>9.8632799999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <f>POWER(2,A3)</f>
+        <v>2048</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1.11182</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1.9565399999999999</v>
+      </c>
+      <c r="E3" s="5">
+        <v>9.8740199999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ref="B4:B22" si="0">POWER(2,A4)</f>
+        <v>4096</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1.11182</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1.9895</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10.0405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="0"/>
+        <v>8192</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1.10938</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2.0019499999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <v>9.9879200000000008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1.1097399999999999</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2.00061</v>
+      </c>
+      <c r="E6" s="5">
+        <v>9.9829699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1.1106</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1.9989300000000001</v>
+      </c>
+      <c r="E7" s="5">
+        <v>9.9491300000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1.11103</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2.0003500000000001</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9.9352499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>131072</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1.1116299999999999</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1.9974400000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <v>9.9272200000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1.1115900000000001</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1.9946200000000001</v>
+      </c>
+      <c r="E10" s="5">
+        <v>9.9206599999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1.11148</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1.9947999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>1048576</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1.1114999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>2097152</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1.1115900000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>4194304</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1.1115699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>8388608</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1.1115600000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4">
+        <v>28</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>268435456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="0"/>
+        <v>536870912</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="0"/>
+        <v>1073741824</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D344B96-D6CB-4748-898D-C63129E9C762}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>10</v>
       </c>
       <c r="B2" s="1">
+        <f>POWER(2,A2)</f>
         <v>1024</v>
       </c>
       <c r="C2" s="1">
@@ -19536,12 +21798,16 @@
       <c r="D2" s="1">
         <v>1024</v>
       </c>
+      <c r="E2" s="1">
+        <v>1024</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>11</v>
       </c>
       <c r="B3" s="1">
+        <f>POWER(2,A3)</f>
         <v>2048</v>
       </c>
       <c r="C3" s="1">
@@ -19550,12 +21816,16 @@
       <c r="D3" s="1">
         <v>2048</v>
       </c>
+      <c r="E3" s="1">
+        <v>2048</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>12</v>
       </c>
       <c r="B4" s="1">
+        <f t="shared" ref="B4:B22" si="0">POWER(2,A4)</f>
         <v>4096</v>
       </c>
       <c r="C4" s="1">
@@ -19564,12 +21834,16 @@
       <c r="D4" s="1">
         <v>4096</v>
       </c>
+      <c r="E4" s="1">
+        <v>4096</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>13</v>
       </c>
       <c r="B5" s="1">
+        <f t="shared" si="0"/>
         <v>8192</v>
       </c>
       <c r="C5" s="1">
@@ -19578,12 +21852,16 @@
       <c r="D5" s="1">
         <v>8192</v>
       </c>
+      <c r="E5" s="1">
+        <v>8192</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>14</v>
       </c>
       <c r="B6" s="1">
+        <f t="shared" si="0"/>
         <v>16384</v>
       </c>
       <c r="C6" s="1">
@@ -19592,12 +21870,16 @@
       <c r="D6" s="1">
         <v>16384</v>
       </c>
+      <c r="E6" s="1">
+        <v>16384</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>15</v>
       </c>
       <c r="B7" s="1">
+        <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="C7" s="1">
@@ -19606,85 +21888,193 @@
       <c r="D7" s="1">
         <v>32768</v>
       </c>
+      <c r="E7" s="1">
+        <v>32768</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>16</v>
       </c>
       <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+      <c r="C8" s="1">
         <v>65533</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>65535</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>65534</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>17</v>
       </c>
       <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>131072</v>
+      </c>
+      <c r="C9" s="1">
         <v>131067</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>131069</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>131066</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>18</v>
       </c>
       <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>262144</v>
+      </c>
+      <c r="C10" s="1">
         <v>262115</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>262109</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>262110</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>19</v>
       </c>
       <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>524288</v>
+      </c>
+      <c r="C11" s="1">
         <v>524151</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>524171</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>1048080</v>
+        <f t="shared" si="0"/>
+        <v>1048576</v>
       </c>
       <c r="C12" s="1">
         <v>1048080</v>
       </c>
+      <c r="D12" s="1">
+        <v>1048080</v>
+      </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>21</v>
       </c>
       <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>2097152</v>
+      </c>
+      <c r="C13" s="1">
         <v>2095020</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>22</v>
       </c>
       <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>4194304</v>
+      </c>
+      <c r="C14" s="1">
         <v>4186020</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>268435456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>536870912</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>1073741824</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>